<commit_message>
Prog RFID + ESP + rapport
</commit_message>
<xml_diff>
--- a/doc/planification/2312_BadgePlace_Planing.xlsx
+++ b/doc/planification/2312_BadgePlace_Planing.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ETML-ES\2312_BadgePlace\doc\planification\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\microchip\harmony\v2_06\apps\2312_BadgePlace\doc\planification\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F869DAF-A42F-4ED1-85C2-4A19665A3C07}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840"/>
   </bookViews>
   <sheets>
     <sheet name="2312_Planning" sheetId="1" r:id="rId1"/>
@@ -110,7 +109,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -751,6 +750,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -760,8 +761,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1089,14 +1088,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:AX31"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AC8" sqref="AC8"/>
+      <selection activeCell="AP11" sqref="AP11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1258,7 +1257,7 @@
       </c>
     </row>
     <row r="2" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="66" t="s">
         <v>0</v>
       </c>
       <c r="B2" s="27"/>
@@ -1312,7 +1311,7 @@
       <c r="AX2" s="19"/>
     </row>
     <row r="3" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="65"/>
+      <c r="A3" s="67"/>
       <c r="B3" s="29"/>
       <c r="C3" s="30"/>
       <c r="D3" s="30"/>
@@ -1364,7 +1363,7 @@
       <c r="AX3" s="7"/>
     </row>
     <row r="4" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="66" t="s">
         <v>1</v>
       </c>
       <c r="B4" s="20"/>
@@ -1418,7 +1417,7 @@
       <c r="AX4" s="19"/>
     </row>
     <row r="5" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A5" s="65"/>
+      <c r="A5" s="67"/>
       <c r="B5" s="5"/>
       <c r="C5" s="6"/>
       <c r="D5" s="33"/>
@@ -1470,7 +1469,7 @@
       <c r="AX5" s="7"/>
     </row>
     <row r="6" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="64" t="s">
+      <c r="A6" s="66" t="s">
         <v>5</v>
       </c>
       <c r="B6" s="20"/>
@@ -1524,7 +1523,7 @@
       <c r="AX6" s="19"/>
     </row>
     <row r="7" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A7" s="65"/>
+      <c r="A7" s="67"/>
       <c r="B7" s="5"/>
       <c r="C7" s="6"/>
       <c r="D7" s="6"/>
@@ -1576,7 +1575,7 @@
       <c r="AX7" s="7"/>
     </row>
     <row r="8" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="64" t="s">
+      <c r="A8" s="66" t="s">
         <v>3</v>
       </c>
       <c r="B8" s="20"/>
@@ -1630,7 +1629,7 @@
       <c r="AX8" s="19"/>
     </row>
     <row r="9" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="66"/>
+      <c r="A9" s="68"/>
       <c r="B9" s="5"/>
       <c r="C9" s="6"/>
       <c r="D9" s="6"/>
@@ -1682,7 +1681,7 @@
       <c r="AX9" s="7"/>
     </row>
     <row r="10" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="64" t="s">
+      <c r="A10" s="66" t="s">
         <v>2</v>
       </c>
       <c r="B10" s="20"/>
@@ -1736,7 +1735,7 @@
       <c r="AX10" s="19"/>
     </row>
     <row r="11" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="65"/>
+      <c r="A11" s="67"/>
       <c r="B11" s="22"/>
       <c r="C11" s="23"/>
       <c r="D11" s="23"/>
@@ -1788,7 +1787,7 @@
       <c r="AX11" s="24"/>
     </row>
     <row r="12" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="64" t="s">
+      <c r="A12" s="66" t="s">
         <v>6</v>
       </c>
       <c r="B12" s="20"/>
@@ -1842,7 +1841,7 @@
       <c r="AX12" s="19"/>
     </row>
     <row r="13" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="65"/>
+      <c r="A13" s="67"/>
       <c r="B13" s="5"/>
       <c r="C13" s="6"/>
       <c r="D13" s="6"/>
@@ -1894,7 +1893,7 @@
       <c r="AX13" s="7"/>
     </row>
     <row r="14" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="64" t="s">
+      <c r="A14" s="66" t="s">
         <v>4</v>
       </c>
       <c r="B14" s="20"/>
@@ -1948,7 +1947,7 @@
       <c r="AX14" s="19"/>
     </row>
     <row r="15" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A15" s="65"/>
+      <c r="A15" s="67"/>
       <c r="B15" s="5"/>
       <c r="C15" s="6"/>
       <c r="D15" s="6"/>
@@ -2000,7 +1999,7 @@
       <c r="AX15" s="7"/>
     </row>
     <row r="16" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="64" t="s">
+      <c r="A16" s="66" t="s">
         <v>7</v>
       </c>
       <c r="B16" s="20"/>
@@ -2054,7 +2053,7 @@
       <c r="AX16" s="19"/>
     </row>
     <row r="17" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="65"/>
+      <c r="A17" s="67"/>
       <c r="B17" s="5"/>
       <c r="C17" s="6"/>
       <c r="D17" s="6"/>
@@ -2106,7 +2105,7 @@
       <c r="AX17" s="7"/>
     </row>
     <row r="18" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="64" t="s">
+      <c r="A18" s="66" t="s">
         <v>8</v>
       </c>
       <c r="B18" s="20"/>
@@ -2160,7 +2159,7 @@
       <c r="AX18" s="19"/>
     </row>
     <row r="19" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="65"/>
+      <c r="A19" s="67"/>
       <c r="B19" s="5"/>
       <c r="C19" s="6"/>
       <c r="D19" s="6"/>
@@ -2212,7 +2211,7 @@
       <c r="AX19" s="7"/>
     </row>
     <row r="20" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="64" t="s">
+      <c r="A20" s="66" t="s">
         <v>10</v>
       </c>
       <c r="B20" s="20"/>
@@ -2229,8 +2228,8 @@
       <c r="M20" s="18"/>
       <c r="N20" s="18"/>
       <c r="O20" s="19"/>
-      <c r="P20" s="67"/>
-      <c r="Q20" s="68"/>
+      <c r="P20" s="64"/>
+      <c r="Q20" s="65"/>
       <c r="R20" s="51"/>
       <c r="S20" s="51"/>
       <c r="T20" s="51"/>
@@ -2266,7 +2265,7 @@
       <c r="AX20" s="19"/>
     </row>
     <row r="21" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A21" s="65"/>
+      <c r="A21" s="67"/>
       <c r="B21" s="5"/>
       <c r="C21" s="6"/>
       <c r="D21" s="6"/>
@@ -2295,9 +2294,9 @@
       <c r="AA21" s="52"/>
       <c r="AB21" s="6"/>
       <c r="AC21" s="7"/>
-      <c r="AD21" s="5"/>
-      <c r="AE21" s="6"/>
-      <c r="AF21" s="6"/>
+      <c r="AD21" s="52"/>
+      <c r="AE21" s="52"/>
+      <c r="AF21" s="52"/>
       <c r="AG21" s="6"/>
       <c r="AH21" s="6"/>
       <c r="AI21" s="6"/>
@@ -2318,7 +2317,7 @@
       <c r="AX21" s="7"/>
     </row>
     <row r="22" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="64" t="s">
+      <c r="A22" s="66" t="s">
         <v>9</v>
       </c>
       <c r="B22" s="20"/>
@@ -2344,9 +2343,9 @@
       <c r="V22" s="19"/>
       <c r="W22" s="20"/>
       <c r="X22" s="18"/>
-      <c r="Y22" s="68"/>
-      <c r="Z22" s="68"/>
-      <c r="AA22" s="68"/>
+      <c r="Y22" s="65"/>
+      <c r="Z22" s="65"/>
+      <c r="AA22" s="65"/>
       <c r="AB22" s="18"/>
       <c r="AC22" s="19"/>
       <c r="AD22" s="53"/>
@@ -2372,7 +2371,7 @@
       <c r="AX22" s="19"/>
     </row>
     <row r="23" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="65"/>
+      <c r="A23" s="67"/>
       <c r="B23" s="5"/>
       <c r="C23" s="6"/>
       <c r="D23" s="6"/>
@@ -2424,7 +2423,7 @@
       <c r="AX23" s="7"/>
     </row>
     <row r="24" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="64" t="s">
+      <c r="A24" s="66" t="s">
         <v>11</v>
       </c>
       <c r="B24" s="20"/>
@@ -2455,9 +2454,9 @@
       <c r="AA24" s="18"/>
       <c r="AB24" s="18"/>
       <c r="AC24" s="19"/>
-      <c r="AD24" s="67"/>
-      <c r="AE24" s="68"/>
-      <c r="AF24" s="68"/>
+      <c r="AD24" s="64"/>
+      <c r="AE24" s="65"/>
+      <c r="AF24" s="65"/>
       <c r="AG24" s="31"/>
       <c r="AH24" s="31"/>
       <c r="AI24" s="18"/>
@@ -2478,7 +2477,7 @@
       <c r="AX24" s="19"/>
     </row>
     <row r="25" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A25" s="65"/>
+      <c r="A25" s="67"/>
       <c r="B25" s="5"/>
       <c r="C25" s="6"/>
       <c r="D25" s="6"/>
@@ -2530,7 +2529,7 @@
       <c r="AX25" s="7"/>
     </row>
     <row r="26" spans="1:50" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="64" t="s">
+      <c r="A26" s="66" t="s">
         <v>12</v>
       </c>
       <c r="B26" s="54"/>
@@ -2584,7 +2583,7 @@
       <c r="AX26" s="19"/>
     </row>
     <row r="27" spans="1:50" ht="12.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="65"/>
+      <c r="A27" s="67"/>
       <c r="B27" s="5"/>
       <c r="C27" s="6"/>
       <c r="D27" s="6"/>
@@ -2613,9 +2612,9 @@
       <c r="AA27" s="57"/>
       <c r="AB27" s="57"/>
       <c r="AC27" s="58"/>
-      <c r="AD27" s="5"/>
-      <c r="AE27" s="6"/>
-      <c r="AF27" s="6"/>
+      <c r="AD27" s="57"/>
+      <c r="AE27" s="57"/>
+      <c r="AF27" s="57"/>
       <c r="AG27" s="6"/>
       <c r="AH27" s="6"/>
       <c r="AI27" s="6"/>
@@ -2853,12 +2852,6 @@
     </row>
   </sheetData>
   <mergeCells count="13">
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="A10:A11"/>
     <mergeCell ref="A24:A25"/>
     <mergeCell ref="A26:A27"/>
     <mergeCell ref="A14:A15"/>
@@ -2866,10 +2859,16 @@
     <mergeCell ref="A18:A19"/>
     <mergeCell ref="A20:A21"/>
     <mergeCell ref="A22:A23"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="A2:A3"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
+    <mergeCell ref="A10:A11"/>
   </mergeCells>
   <printOptions verticalCentered="1"/>
   <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" fitToWidth="0" orientation="landscape" horizontalDpi="4294967293" r:id="rId1"/>
   <headerFooter>
     <oddHeader>&amp;L2312 Badge pour place de travail&amp;CPlanning&amp;R2023</oddHeader>
     <oddFooter>&amp;LMiguel Santos&amp;CSLO&amp;R&amp;P</oddFooter>

</xml_diff>